<commit_message>
new paper figure versions missing resource maps
</commit_message>
<xml_diff>
--- a/csvs/palette.xlsx
+++ b/csvs/palette.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Guille/Desktop/india_power/gridpath_india_viz/csvs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB4F6B7-2675-E249-9222-3B45864F7E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26553A2-BDA7-8C4D-B826-5A5DD5ADF903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="16080" windowHeight="15960" xr2:uid="{DFF9881E-538D-D94E-B8B3-BDF1B81E3663}"/>
+    <workbookView xWindow="-160" yWindow="2720" windowWidth="16080" windowHeight="15960" xr2:uid="{DFF9881E-538D-D94E-B8B3-BDF1B81E3663}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>#485408</t>
   </si>
@@ -111,6 +111,42 @@
   </si>
   <si>
     <t>dashdotdotted</t>
+  </si>
+  <si>
+    <t>wind</t>
+  </si>
+  <si>
+    <t>solar</t>
+  </si>
+  <si>
+    <t>#c3eff1</t>
+  </si>
+  <si>
+    <t>#90c2ec</t>
+  </si>
+  <si>
+    <t>#4a9ae4</t>
+  </si>
+  <si>
+    <t>#4b69c5</t>
+  </si>
+  <si>
+    <t>#3b3aa5</t>
+  </si>
+  <si>
+    <t>#feeed5</t>
+  </si>
+  <si>
+    <t>#fdd3aa</t>
+  </si>
+  <si>
+    <t>#ffbc85</t>
+  </si>
+  <si>
+    <t>#f8a462</t>
+  </si>
+  <si>
+    <t>#f19139</t>
   </si>
 </sst>
 </file>
@@ -485,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB3FA79-CCAD-D24E-A0CC-656DAA3FCE35}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,7 +533,7 @@
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -510,8 +546,14 @@
       <c r="D1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -524,8 +566,14 @@
       <c r="D2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -538,8 +586,14 @@
       <c r="D3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -552,8 +606,14 @@
       <c r="D4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -566,8 +626,14 @@
       <c r="D5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -577,8 +643,14 @@
       <c r="D6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -586,7 +658,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -594,17 +666,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Buthan added to the graphs
</commit_message>
<xml_diff>
--- a/csvs/palette.xlsx
+++ b/csvs/palette.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Guille/Desktop/india_power/gridpath_india_viz/csvs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26553A2-BDA7-8C4D-B826-5A5DD5ADF903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85266773-A2EA-6042-8833-3F2BCD70944B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-160" yWindow="2720" windowWidth="16080" windowHeight="15960" xr2:uid="{DFF9881E-538D-D94E-B8B3-BDF1B81E3663}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16080" windowHeight="15960" xr2:uid="{DFF9881E-538D-D94E-B8B3-BDF1B81E3663}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -524,7 +524,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -547,10 +547,10 @@
         <v>19</v>
       </c>
       <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
         <v>25</v>
-      </c>
-      <c r="F1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">

</xml_diff>